<commit_message>
Add ability to import existing JSON files
</commit_message>
<xml_diff>
--- a/example/internationalization.xlsx
+++ b/example/internationalization.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="package_settings" sheetId="1" state="visible" r:id="rId2"/>
@@ -36,31 +36,31 @@
     <t xml:space="preserve">key</t>
   </si>
   <si>
-    <t xml:space="preserve">this is the first key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is the first key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Это первый ключ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">this is the second key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is the second key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Это второй ключ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">this is the third key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is the third key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Это третий ключ</t>
+    <t xml:space="preserve">sign-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sign Up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Регистрация</t>
+  </si>
+  <si>
+    <t xml:space="preserve">our-product-heading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is our great product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Это наш великолепный продукт</t>
+  </si>
+  <si>
+    <t xml:space="preserve">footer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Footer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Футер</t>
   </si>
   <si>
     <t xml:space="preserve">this is header key</t>
@@ -91,7 +91,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -113,6 +113,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -164,7 +172,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -173,11 +181,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -200,11 +212,11 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.65"/>
   </cols>
@@ -238,15 +250,15 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="28.7"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="1" width="12.63"/>
   </cols>
   <sheetData>
@@ -262,21 +274,21 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -284,10 +296,10 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -296,7 +308,7 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -316,39 +328,39 @@
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -362,7 +374,7 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>

</xml_diff>